<commit_message>
Added missing component and connections
</commit_message>
<xml_diff>
--- a/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-DigiKey.xlsx
+++ b/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-DigiKey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/PCBWay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/BOMs/PCBWay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADFAB16-DF92-FB49-AE5D-997C93B38EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46C30C3-2646-0145-AB39-95D9DD9D7AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>DigiKey Part: WM11263CT-ND</t>
   </si>
   <si>
-    <t>C1,C2</t>
-  </si>
-  <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>HYBRID</t>
+  </si>
+  <si>
+    <t>C1,C2,C11</t>
   </si>
 </sst>
 </file>
@@ -920,7 +920,7 @@
   <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -941,7 +941,7 @@
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="D2" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
@@ -1010,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>16</v>
@@ -1021,28 +1021,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="F8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="G8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="18" t="s">
-        <v>43</v>
-      </c>
       <c r="H8" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1050,28 +1050,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="F9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="H9" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1085,22 +1085,22 @@
         <v>1</v>
       </c>
       <c r="D10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="F10" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="G10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1108,28 +1108,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="22">
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="G11" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>53</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1137,28 +1137,28 @@
         <v>6</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="22">
         <v>1</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="F12" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="G12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1166,28 +1166,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="22">
         <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="F13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="H13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>64</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1195,28 +1195,28 @@
         <v>8</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="15">
-        <v>2</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="H14" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>21</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1224,28 +1224,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="13">
         <v>4</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="G15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1">
@@ -1253,28 +1253,28 @@
         <v>10</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="13">
         <v>2</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="G16" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1282,28 +1282,28 @@
         <v>11</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="13">
         <v>2</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="G17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1311,28 +1311,28 @@
         <v>12</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="13">
         <v>2</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="F18" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="G18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1340,28 +1340,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1369,28 +1369,28 @@
         <v>14</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="13">
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="G20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1398,28 +1398,28 @@
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="13">
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="G21" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9">

</xml_diff>

<commit_message>
New board layout.  Made things smaller, removed large trenches, and calculated USB differential impedance.
</commit_message>
<xml_diff>
--- a/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-DigiKey.xlsx
+++ b/Production/BOMs/PCBWay/3DProUsb-PCBWay-BOM-DigiKey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kreeblah/SidewinderToUSBV2/Production/BOMs/PCBWay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46C30C3-2646-0145-AB39-95D9DD9D7AFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F61C31-4B25-4841-9375-78C962233FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
   <si>
     <t>Item #</t>
   </si>
@@ -129,9 +129,6 @@
     <t>SMD</t>
   </si>
   <si>
-    <t>Molex</t>
-  </si>
-  <si>
     <t>Need a quick and accurante quote? Need an efficient production? Please read SMT Ordering Necessary Files &amp; Info in 1 minute. Thank you very much!</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
   </si>
   <si>
-    <t>DigiKey Part: WM11263CT-ND</t>
-  </si>
-  <si>
     <t>Taiyo Yuden</t>
   </si>
   <si>
@@ -355,6 +349,15 @@
   </si>
   <si>
     <t>C1,C2,C11</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>10118193-0001LF</t>
+  </si>
+  <si>
+    <t>DigiKey Part: 609-4616-2-ND</t>
   </si>
 </sst>
 </file>
@@ -941,7 +944,7 @@
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="D2" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
@@ -992,28 +995,28 @@
         <v>1</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="13">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="14">
-        <v>1051640001</v>
+        <v>85</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
@@ -1021,28 +1024,28 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="17">
         <v>1</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="G8" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>42</v>
-      </c>
       <c r="H8" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1050,28 +1053,28 @@
         <v>3</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
       </c>
       <c r="D9" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="G9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="H9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1085,22 +1088,22 @@
         <v>1</v>
       </c>
       <c r="D10" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="G10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="20" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1108,28 +1111,28 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C11" s="22">
         <v>1</v>
       </c>
       <c r="D11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="G11" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1137,28 +1140,28 @@
         <v>6</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="22">
         <v>1</v>
       </c>
       <c r="D12" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="G12" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1166,28 +1169,28 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="22">
         <v>1</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="G13" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="H13" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="21" t="s">
         <v>62</v>
-      </c>
-      <c r="G13" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1195,28 +1198,28 @@
         <v>8</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="G14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="H14" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>19</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1224,28 +1227,28 @@
         <v>9</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="13">
         <v>4</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E15" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1">
@@ -1253,28 +1256,28 @@
         <v>10</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="13">
         <v>2</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1282,28 +1285,28 @@
         <v>11</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="13">
         <v>2</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1311,28 +1314,28 @@
         <v>12</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="13">
         <v>2</v>
       </c>
       <c r="D18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="G18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1340,28 +1343,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="13">
         <v>2</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1369,28 +1372,28 @@
         <v>14</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="13">
         <v>2</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1398,33 +1401,33 @@
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C21" s="13">
         <v>1</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="H21" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1448,7 +1451,7 @@
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1">
       <c r="A26" s="25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="25"/>

</xml_diff>